<commit_message>
doc: Add JavaDoc for read cases (#301)
</commit_message>
<xml_diff>
--- a/fastexcel-test/src/test/resources/demo/demo.xlsx
+++ b/fastexcel-test/src/test/resources/demo/demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanxin/Documents/GitHub/fastexcel/fastexcel-test/src/test/resources/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFF7C4D-47FE-DD47-808C-C06FCFD33AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C06F3A7-DF50-654E-AB3F-5E495B027276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="3700" windowWidth="28800" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3700" windowWidth="28800" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,46 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t>字符串标题</t>
-  </si>
-  <si>
-    <t>日期标题</t>
-  </si>
-  <si>
-    <t>数字标题</t>
-  </si>
-  <si>
-    <t>表2字符串0</t>
-  </si>
-  <si>
-    <t>表2字符串1</t>
-  </si>
-  <si>
-    <t>表2字符串2</t>
-  </si>
-  <si>
-    <t>表2字符串3</t>
-  </si>
-  <si>
-    <t>表2字符串4</t>
-  </si>
-  <si>
-    <t>表2字符串5</t>
-  </si>
-  <si>
-    <t>表2字符串6</t>
-  </si>
-  <si>
-    <t>表2字符串7</t>
-  </si>
-  <si>
-    <t>表2字符串8</t>
-  </si>
-  <si>
-    <t>表2字符串9</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -104,6 +65,38 @@
   </si>
   <si>
     <t>String9</t>
+  </si>
+  <si>
+    <t>Table 2 String 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Table 2 String 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Table 2 String 2</t>
+  </si>
+  <si>
+    <t>Table 2 String 3</t>
+  </si>
+  <si>
+    <t>Table 2 String 4</t>
+  </si>
+  <si>
+    <t>Table 2 String 5</t>
+  </si>
+  <si>
+    <t>Table 2 String 6</t>
+  </si>
+  <si>
+    <t>Table 2 String 7</t>
+  </si>
+  <si>
+    <t>Table 2 String 8</t>
+  </si>
+  <si>
+    <t>Table 2 String 9</t>
   </si>
 </sst>
 </file>
@@ -156,11 +149,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -479,7 +469,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -490,21 +480,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>14</v>
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
         <v>43831.042372685202</v>
       </c>
       <c r="C2">
@@ -512,10 +502,10 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
         <v>43832.042372685202</v>
       </c>
       <c r="C3">
@@ -523,10 +513,10 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
         <v>43833.042372685202</v>
       </c>
       <c r="C4">
@@ -534,10 +524,10 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
         <v>43834.042372685202</v>
       </c>
       <c r="C5">
@@ -545,10 +535,10 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
         <v>43835.042372685202</v>
       </c>
       <c r="C6">
@@ -556,10 +546,10 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
         <v>43836.042372685202</v>
       </c>
       <c r="C7">
@@ -567,10 +557,10 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
         <v>43837.042372685202</v>
       </c>
       <c r="C8">
@@ -578,10 +568,10 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
         <v>43838.042372685202</v>
       </c>
       <c r="C9">
@@ -589,10 +579,10 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
         <v>43839.042372685202</v>
       </c>
       <c r="C10">
@@ -600,10 +590,10 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="2">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
         <v>43840.042372685202</v>
       </c>
       <c r="C11">
@@ -622,27 +612,31 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1">
         <v>43831.042372685202</v>
       </c>
       <c r="C2">
@@ -650,10 +644,10 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1">
         <v>43832.042372685202</v>
       </c>
       <c r="C3">
@@ -661,10 +655,10 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1">
         <v>43833.042372685202</v>
       </c>
       <c r="C4">
@@ -672,10 +666,10 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1">
         <v>43834.042372685202</v>
       </c>
       <c r="C5">
@@ -683,10 +677,10 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1">
         <v>43835.042372685202</v>
       </c>
       <c r="C6">
@@ -694,10 +688,10 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1">
         <v>43836.042372685202</v>
       </c>
       <c r="C7">
@@ -705,10 +699,10 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1">
         <v>43837.042372685202</v>
       </c>
       <c r="C8">
@@ -716,10 +710,10 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1">
         <v>43838.042372685202</v>
       </c>
       <c r="C9">
@@ -727,10 +721,10 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="A10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1">
         <v>43839.042372685202</v>
       </c>
       <c r="C10">
@@ -738,10 +732,10 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="2">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1">
         <v>43840.042372685202</v>
       </c>
       <c r="C11">

</xml_diff>